<commit_message>
Moved manta in CLR from scientific name to topic
</commit_message>
<xml_diff>
--- a/datamares/CLR/CLR_datamares_manta.xlsx
+++ b/datamares/CLR/CLR_datamares_manta.xlsx
@@ -2984,8 +2984,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3050,7 +3050,7 @@
         <v>353</v>
       </c>
       <c r="O1" s="16" t="s">
-        <v>509</v>
+        <v>459</v>
       </c>
       <c r="P1" s="16" t="s">
         <v>454</v>

</xml_diff>

<commit_message>
Updated OLRs and a CLR based on QA
</commit_message>
<xml_diff>
--- a/datamares/CLR/CLR_datamares_manta.xlsx
+++ b/datamares/CLR/CLR_datamares_manta.xlsx
@@ -2984,8 +2984,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>